<commit_message>
Implementação de arquivo com 129 instâncias escolares (cont.)
</commit_message>
<xml_diff>
--- a/Relatório final 129 instâncias.xlsx
+++ b/Relatório final 129 instâncias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edmilson1\Documents\UFSC\UFSC - curso de Sistemas de Informação 2019.2\Fase 8\TCC_Edmilson-Domingues\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514E81BC-31D2-4C02-AD68-1D5F00BCFB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36ADF02E-5802-44DE-B869-E397EF706615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9AAF1EFB-0EF3-415D-937B-D7B9DFA7D6DF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="66">
   <si>
     <t>Código</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t>EEB PROF ALEXANDRE SERGIO GODINHO</t>
+  </si>
+  <si>
+    <t>EEB PREF AVELINO MULLER</t>
+  </si>
+  <si>
+    <t>EEB DR ADERBAL RAMOS DA SILVA</t>
   </si>
 </sst>
 </file>
@@ -599,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C54A5B6D-8B78-4410-B9E0-983D5544B74F}">
   <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2698,15 +2704,105 @@
       <c r="B43">
         <v>2720</v>
       </c>
+      <c r="C43" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D43" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43">
+        <v>20</v>
+      </c>
+      <c r="I43">
+        <v>47</v>
+      </c>
+      <c r="J43">
+        <v>23</v>
+      </c>
+      <c r="K43">
+        <v>50</v>
+      </c>
+      <c r="L43">
+        <v>28</v>
+      </c>
+      <c r="M43">
+        <v>3000</v>
+      </c>
+      <c r="N43">
+        <v>50</v>
+      </c>
+      <c r="O43">
+        <v>555</v>
+      </c>
+      <c r="P43">
+        <v>3</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
+      <c r="B44">
+        <v>2674</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" t="s">
+        <v>11</v>
+      </c>
+      <c r="H44">
+        <v>26</v>
+      </c>
+      <c r="I44">
+        <v>47</v>
+      </c>
+      <c r="J44">
+        <v>22</v>
+      </c>
+      <c r="K44">
+        <v>50</v>
+      </c>
+      <c r="L44">
+        <v>15</v>
+      </c>
+      <c r="M44">
+        <v>3550</v>
+      </c>
+      <c r="N44">
+        <v>592</v>
+      </c>
+      <c r="O44">
+        <v>585</v>
+      </c>
+      <c r="P44">
+        <v>4</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
+      </c>
+      <c r="B45">
+        <v>2739</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Implementação outros turnos em AG (cont.)
</commit_message>
<xml_diff>
--- a/Relatório final 129 instâncias.xlsx
+++ b/Relatório final 129 instâncias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edmilson1\Documents\UFSC\UFSC - curso de Sistemas de Informação 2019.2\Fase 8\TCC_Edmilson-Domingues\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF554300-01D0-456C-B151-C158BCCCE1F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F640CE78-CF7C-4AB1-B4F0-EA4439C4DA7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9AAF1EFB-0EF3-415D-937B-D7B9DFA7D6DF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="162">
   <si>
     <t>Código</t>
   </si>
@@ -487,6 +487,30 @@
   </si>
   <si>
     <t>Não sai do 125/150</t>
+  </si>
+  <si>
+    <t>Não saía da turma 16</t>
+  </si>
+  <si>
+    <t>Não saía da turma 18</t>
+  </si>
+  <si>
+    <t>Fazer de madrugada</t>
+  </si>
+  <si>
+    <t>Não saía da turma 21</t>
+  </si>
+  <si>
+    <t>Não sai do 125/150 - turma 13</t>
+  </si>
+  <si>
+    <t>Não sai do 147/150 - turma 8</t>
+  </si>
+  <si>
+    <t>Não sai do 125/150 turma 8</t>
+  </si>
+  <si>
+    <t>Não sai do 149/150 na turma 21</t>
   </si>
 </sst>
 </file>
@@ -893,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C54A5B6D-8B78-4410-B9E0-983D5544B74F}">
   <dimension ref="A1:Y137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3318,6 +3342,21 @@
       <c r="Q40" t="s">
         <v>9</v>
       </c>
+      <c r="T40">
+        <v>12.19</v>
+      </c>
+      <c r="U40">
+        <v>533</v>
+      </c>
+      <c r="V40">
+        <v>450</v>
+      </c>
+      <c r="W40">
+        <v>33</v>
+      </c>
+      <c r="X40" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41">
@@ -3365,6 +3404,21 @@
       <c r="Q41" t="s">
         <v>9</v>
       </c>
+      <c r="T41">
+        <v>11.85</v>
+      </c>
+      <c r="U41">
+        <v>452</v>
+      </c>
+      <c r="V41">
+        <v>441</v>
+      </c>
+      <c r="W41">
+        <v>34</v>
+      </c>
+      <c r="X41" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42">
@@ -3412,13 +3466,28 @@
       <c r="Q42" t="s">
         <v>9</v>
       </c>
+      <c r="T42">
+        <v>13.53</v>
+      </c>
+      <c r="U42">
+        <v>571</v>
+      </c>
+      <c r="V42">
+        <v>455</v>
+      </c>
+      <c r="W42">
+        <v>37</v>
+      </c>
+      <c r="X42" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>6</v>
       </c>
       <c r="B43">
-        <v>710</v>
+        <v>744</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>13</v>
@@ -3458,6 +3527,9 @@
       </c>
       <c r="Q43" t="s">
         <v>9</v>
+      </c>
+      <c r="X43" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
@@ -3512,6 +3584,21 @@
       <c r="Q44" t="s">
         <v>9</v>
       </c>
+      <c r="T44">
+        <v>12.14</v>
+      </c>
+      <c r="U44">
+        <v>331</v>
+      </c>
+      <c r="V44">
+        <v>477</v>
+      </c>
+      <c r="W44">
+        <v>48</v>
+      </c>
+      <c r="X44" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45">
@@ -3559,6 +3646,9 @@
       <c r="Q45" t="s">
         <v>9</v>
       </c>
+      <c r="X45" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46">
@@ -3609,6 +3699,21 @@
       <c r="Q46" t="s">
         <v>9</v>
       </c>
+      <c r="T46">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="U46">
+        <v>140</v>
+      </c>
+      <c r="V46">
+        <v>316</v>
+      </c>
+      <c r="W46">
+        <v>26</v>
+      </c>
+      <c r="X46" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47">
@@ -3659,6 +3764,21 @@
       <c r="Q47" t="s">
         <v>9</v>
       </c>
+      <c r="T47">
+        <v>16.190000000000001</v>
+      </c>
+      <c r="U47">
+        <v>575</v>
+      </c>
+      <c r="V47">
+        <v>491</v>
+      </c>
+      <c r="W47">
+        <v>46</v>
+      </c>
+      <c r="X47" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48">
@@ -3706,8 +3826,23 @@
       <c r="Q48" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T48">
+        <v>20.48</v>
+      </c>
+      <c r="U48">
+        <v>669</v>
+      </c>
+      <c r="V48">
+        <v>442</v>
+      </c>
+      <c r="W48">
+        <v>36</v>
+      </c>
+      <c r="X48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>23</v>
       </c>
@@ -3753,8 +3888,23 @@
       <c r="Q49" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T49">
+        <v>19.88</v>
+      </c>
+      <c r="U49">
+        <v>786</v>
+      </c>
+      <c r="V49">
+        <v>519</v>
+      </c>
+      <c r="W49">
+        <v>52</v>
+      </c>
+      <c r="X49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>13</v>
       </c>
@@ -3800,8 +3950,11 @@
       <c r="Q50" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="X50" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>66</v>
       </c>
@@ -3853,8 +4006,11 @@
       <c r="Q51" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="X51" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>25</v>
       </c>
@@ -3900,8 +4056,11 @@
       <c r="Q52" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="X52" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>28</v>
       </c>
@@ -3947,8 +4106,11 @@
       <c r="Q53" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="X53" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>87</v>
       </c>
@@ -4000,8 +4162,23 @@
       <c r="Q54" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T54">
+        <v>6.5</v>
+      </c>
+      <c r="U54">
+        <v>320</v>
+      </c>
+      <c r="V54">
+        <v>421</v>
+      </c>
+      <c r="W54">
+        <v>33</v>
+      </c>
+      <c r="X54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>89</v>
       </c>
@@ -4050,8 +4227,11 @@
       <c r="Q55" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="X55" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>41</v>
       </c>
@@ -4097,8 +4277,11 @@
       <c r="Q56" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="X56" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>51</v>
       </c>
@@ -4150,8 +4333,23 @@
       <c r="Q57" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T57">
+        <v>16.32</v>
+      </c>
+      <c r="U57">
+        <v>359</v>
+      </c>
+      <c r="V57">
+        <v>602</v>
+      </c>
+      <c r="W57">
+        <v>59</v>
+      </c>
+      <c r="X57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>53</v>
       </c>
@@ -4203,8 +4401,23 @@
       <c r="Q58" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T58">
+        <v>38.47</v>
+      </c>
+      <c r="U58">
+        <v>672</v>
+      </c>
+      <c r="V58">
+        <v>651</v>
+      </c>
+      <c r="W58">
+        <v>83</v>
+      </c>
+      <c r="X58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>68</v>
       </c>
@@ -4250,8 +4463,23 @@
       <c r="Q59" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T59">
+        <v>63.04</v>
+      </c>
+      <c r="U59">
+        <v>1543</v>
+      </c>
+      <c r="V59">
+        <v>600</v>
+      </c>
+      <c r="W59">
+        <v>46</v>
+      </c>
+      <c r="X59" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>74</v>
       </c>
@@ -4297,8 +4525,23 @@
       <c r="Q60" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T60">
+        <v>10.57</v>
+      </c>
+      <c r="U60">
+        <v>469</v>
+      </c>
+      <c r="V60">
+        <v>567</v>
+      </c>
+      <c r="W60">
+        <v>48</v>
+      </c>
+      <c r="X60" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>82</v>
       </c>
@@ -4350,8 +4593,11 @@
       <c r="Q61" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="X61" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>30</v>
       </c>
@@ -4397,8 +4643,11 @@
       <c r="Q62" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="X62" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>40</v>
       </c>
@@ -4447,8 +4696,23 @@
       <c r="Q63" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T63">
+        <v>12.84</v>
+      </c>
+      <c r="U63">
+        <v>359</v>
+      </c>
+      <c r="V63">
+        <v>597</v>
+      </c>
+      <c r="W63">
+        <v>59</v>
+      </c>
+      <c r="X63" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>84</v>
       </c>
@@ -4497,8 +4761,11 @@
       <c r="Q64" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="X64" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>21</v>
       </c>
@@ -4547,8 +4814,23 @@
       <c r="Q65" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T65">
+        <v>9.2200000000000006</v>
+      </c>
+      <c r="U65">
+        <v>219</v>
+      </c>
+      <c r="V65">
+        <v>567</v>
+      </c>
+      <c r="W65">
+        <v>66</v>
+      </c>
+      <c r="X65" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>44</v>
       </c>
@@ -4594,8 +4876,23 @@
       <c r="Q66" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T66">
+        <v>33.130000000000003</v>
+      </c>
+      <c r="U66">
+        <v>1205</v>
+      </c>
+      <c r="V66">
+        <v>592</v>
+      </c>
+      <c r="W66">
+        <v>43</v>
+      </c>
+      <c r="X66" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>50</v>
       </c>
@@ -4647,8 +4944,23 @@
       <c r="Q67" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T67">
+        <v>16.559999999999999</v>
+      </c>
+      <c r="U67">
+        <v>454</v>
+      </c>
+      <c r="V67">
+        <v>616</v>
+      </c>
+      <c r="W67">
+        <v>57</v>
+      </c>
+      <c r="X67" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>88</v>
       </c>
@@ -4698,7 +5010,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>114</v>
       </c>
@@ -4742,7 +5054,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>57</v>
       </c>
@@ -4789,7 +5101,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>49</v>
       </c>
@@ -4839,7 +5151,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>18</v>
       </c>
@@ -4889,7 +5201,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>58</v>
       </c>
@@ -4936,7 +5248,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>54</v>
       </c>
@@ -4983,7 +5295,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>16</v>
       </c>
@@ -5033,7 +5345,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>62</v>
       </c>
@@ -5086,7 +5398,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>63</v>
       </c>
@@ -5133,7 +5445,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>117</v>
       </c>
@@ -5177,7 +5489,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>48</v>
       </c>
@@ -5227,7 +5539,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>3</v>
       </c>
@@ -5277,7 +5589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>75</v>
       </c>
@@ -5324,7 +5636,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>98</v>
       </c>
@@ -5371,7 +5683,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>93</v>
       </c>
@@ -5424,7 +5736,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>8</v>
       </c>
@@ -5477,7 +5789,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>72</v>
       </c>
@@ -5530,7 +5842,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>108</v>
       </c>
@@ -5580,7 +5892,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2</v>
       </c>
@@ -5630,7 +5942,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>67</v>
       </c>
@@ -5683,7 +5995,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>9</v>
       </c>
@@ -5736,7 +6048,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>73</v>
       </c>
@@ -5789,7 +6101,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>80</v>
       </c>
@@ -5836,7 +6148,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>33</v>
       </c>
@@ -5889,7 +6201,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>5</v>
       </c>
@@ -5941,8 +6253,23 @@
       <c r="Q93" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T93">
+        <v>27.89</v>
+      </c>
+      <c r="U93">
+        <v>719</v>
+      </c>
+      <c r="V93">
+        <v>920</v>
+      </c>
+      <c r="W93">
+        <v>79</v>
+      </c>
+      <c r="X93" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>46</v>
       </c>
@@ -5995,7 +6322,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>76</v>
       </c>
@@ -6048,7 +6375,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Implementação da parte de otimização (liberação gradual de janelas)
</commit_message>
<xml_diff>
--- a/Relatório final 129 instâncias.xlsx
+++ b/Relatório final 129 instâncias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edmilson1\Documents\UFSC\UFSC - curso de Sistemas de Informação 2019.2\Fase 8\TCC_Edmilson-Domingues\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450550BE-AF09-4127-8B92-17C7796B9E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD38F6B-4184-4C9D-8019-B12170E1811B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9AAF1EFB-0EF3-415D-937B-D7B9DFA7D6DF}"/>
   </bookViews>
@@ -956,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C54A5B6D-8B78-4410-B9E0-983D5544B74F}">
   <dimension ref="A1:Y137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T99" sqref="T99"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P47" sqref="P47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Inclusão horários nas grades
</commit_message>
<xml_diff>
--- a/Relatório final 129 instâncias.xlsx
+++ b/Relatório final 129 instâncias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edmilson1\Documents\UFSC\UFSC - curso de Sistemas de Informação 2019.2\Fase 8\TCC_Edmilson-Domingues\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D57AFC4-E375-4E49-B370-8C6ADD091630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92CFCBF-5610-4C4B-AC88-B749D621C586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="6" activeTab="9" xr2:uid="{9AAF1EFB-0EF3-415D-937B-D7B9DFA7D6DF}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="7" xr2:uid="{9AAF1EFB-0EF3-415D-937B-D7B9DFA7D6DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Geral" sheetId="1" r:id="rId1"/>
@@ -870,32 +870,9 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2137,32 +2114,9 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2913,32 +2867,9 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -5432,32 +5363,9 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -6226,32 +6134,9 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -7979,7 +7864,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-BR"/>
-              <a:t>Processamento</a:t>
+              <a:t>Número de indivíduos</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -18462,8 +18347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C54A5B6D-8B78-4410-B9E0-983D5544B74F}">
   <dimension ref="A1:Y137"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+    <sheetView topLeftCell="A70" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P81" sqref="P81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27102,8 +26987,8 @@
     </row>
     <row r="137" spans="1:25" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y139">
-    <sortCondition descending="1" ref="P2:P139"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y130">
+    <sortCondition descending="1" ref="P2:P130"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -27115,7 +27000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF47BCA1-A7C1-4D1B-BCF2-F3290BA24014}">
   <dimension ref="A1:AB44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -30119,7 +30004,7 @@
   <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40953,7 +40838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4561894D-3F14-45AD-96E8-CDD4C239C9B2}">
   <dimension ref="A1:Y137"/>
   <sheetViews>
-    <sheetView topLeftCell="M115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M115" workbookViewId="0">
       <selection activeCell="N129" sqref="N129"/>
     </sheetView>
   </sheetViews>

</xml_diff>